<commit_message>
Export cost issues to Excel
</commit_message>
<xml_diff>
--- a/storage/templates/cost-issue-log.xlsx
+++ b/storage/templates/cost-issue-log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="24560" windowHeight="14240" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="24560" windowHeight="14240" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="10" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Project</t>
   </si>
@@ -104,13 +104,65 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Store Resource Code</t>
+  </si>
+  <si>
+    <t>Store Cost</t>
+  </si>
+  <si>
+    <t>Cost Account</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Price/Unit</t>
+  </si>
+  <si>
+    <t>Group / C.C.</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>Item Desc</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>ITEM CODES</t>
+  </si>
+  <si>
+    <t>Doc #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +189,22 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,35 +287,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,9 +351,29 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,13 +662,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -623,6 +711,15 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -635,8 +732,18 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -644,65 +751,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19" style="12" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="15" style="15" customWidth="1"/>
-    <col min="9" max="9" width="18" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="57.33203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="19" style="11" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15" style="14" customWidth="1"/>
+    <col min="9" max="9" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="22"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -713,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -723,12 +830,59 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="25" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="14" style="23" customWidth="1"/>
+    <col min="10" max="10" width="15" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -752,22 +906,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -788,33 +942,33 @@
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -825,12 +979,53 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="7" width="18.6640625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>